<commit_message>
search description in source and wirte into target
</commit_message>
<xml_diff>
--- a/source/input_short_header.xlsx
+++ b/source/input_short_header.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\工作\SCID工具开发\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Coding\SCID_AutoFill\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B3F137-B0CD-4D86-BADB-7298C3B61416}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982030B6-A48A-4104-80CE-1B3B9F7DB31E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16185" windowHeight="6158" xr2:uid="{651EEE8A-6779-41A8-B2F7-3B4EA6DFE9A4}"/>
   </bookViews>
@@ -70,9 +70,6 @@
     <t>Local</t>
   </si>
   <si>
-    <t xml:space="preserve">YASG1001CG- </t>
-  </si>
-  <si>
     <t>---</t>
   </si>
   <si>
@@ -207,6 +204,10 @@
       <t>ASG TRAIN A ON SG1
 UNUSABLE MANUAL SET</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">YASG1001CG- </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -622,6 +623,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
   <cols>
+    <col min="1" max="1" width="49.06640625" customWidth="1"/>
     <col min="3" max="3" width="85.46484375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -639,7 +641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45">
+    <row r="2" spans="1:6" ht="30">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -661,42 +663,42 @@
     </row>
     <row r="3" spans="1:6" ht="62.65">
       <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="62.65">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="203.25">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>